<commit_message>
Updated scripts for nicer code. Added code to calculate BF01 for Table 3.
</commit_message>
<xml_diff>
--- a/Table3_Adachi-and-others.xlsx
+++ b/Table3_Adachi-and-others.xlsx
@@ -269,6 +269,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -277,9 +280,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,12 +585,12 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -638,16 +638,16 @@
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="14">
         <v>0.22</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="14">
         <v>100</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="16">
         <v>18.84</v>
       </c>
     </row>
@@ -655,10 +655,10 @@
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -821,16 +821,16 @@
       <c r="A16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="14">
         <v>0.03</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="14">
         <v>60</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="16">
         <v>0.37</v>
       </c>
     </row>
@@ -838,10 +838,10 @@
       <c r="A17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13"/>
-      <c r="F17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="14"/>
+      <c r="F17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
@@ -882,7 +882,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tidied up helper functions. Updated Table 3. Began updating Table 4 but functions don't return negative correlation r. THIS IS A VERY SERIOUS PROBLEM WHEN CALCULATING BF02.
</commit_message>
<xml_diff>
--- a/Table3_Adachi-and-others.xlsx
+++ b/Table3_Adachi-and-others.xlsx
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -263,9 +263,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -278,8 +275,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,6 +627,7 @@
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="15"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,33 +643,38 @@
       <c r="D3" s="9">
         <v>2513</v>
       </c>
+      <c r="E3" s="16"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.22</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>100</v>
       </c>
-      <c r="F4" s="16">
-        <v>18.84</v>
+      <c r="E4" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="F4" s="19">
+        <v>0.12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="14"/>
-      <c r="F5" s="16"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -673,8 +689,11 @@
       <c r="D6" s="9">
         <v>99</v>
       </c>
-      <c r="F6" s="11">
-        <v>0.02</v>
+      <c r="E6" s="16">
+        <v>2.97</v>
+      </c>
+      <c r="F6" s="18">
+        <v>62.8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -690,8 +709,11 @@
       <c r="D7" s="9">
         <v>101</v>
       </c>
-      <c r="F7" s="11">
-        <v>0.17</v>
+      <c r="E7" s="16">
+        <v>2.34</v>
+      </c>
+      <c r="F7" s="18">
+        <v>7.05</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,15 +729,19 @@
       <c r="D8" s="9">
         <v>120</v>
       </c>
-      <c r="F8" s="11">
-        <v>0.61</v>
+      <c r="E8" s="16">
+        <v>1.44</v>
+      </c>
+      <c r="F8" s="18">
+        <v>1.82</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -730,7 +756,8 @@
       <c r="D10" s="9">
         <v>1454</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -745,8 +772,11 @@
       <c r="D11" s="9">
         <v>84</v>
       </c>
-      <c r="F11" s="11">
-        <v>5.12</v>
+      <c r="E11" s="16">
+        <v>0.79</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,8 +792,11 @@
       <c r="D12" s="9">
         <v>84</v>
       </c>
-      <c r="F12" s="11">
-        <v>1.1100000000000001</v>
+      <c r="E12" s="16">
+        <v>1.93</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,8 +812,11 @@
       <c r="D13" s="9">
         <v>50</v>
       </c>
-      <c r="F13" s="11">
-        <v>0.41</v>
+      <c r="E13" s="16">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="F13" s="18">
+        <v>2.35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,8 +832,11 @@
       <c r="D14" s="9">
         <v>77</v>
       </c>
-      <c r="F14" s="11">
-        <v>0.2</v>
+      <c r="E14" s="16">
+        <v>2.7</v>
+      </c>
+      <c r="F14" s="18">
+        <v>4.37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,41 +852,49 @@
       <c r="D15" s="9">
         <v>42</v>
       </c>
-      <c r="F15" s="11">
-        <v>0.38</v>
+      <c r="E15" s="16">
+        <v>2.21</v>
+      </c>
+      <c r="F15" s="18">
+        <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <v>0.03</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>60</v>
       </c>
-      <c r="F16" s="16">
-        <v>0.37</v>
+      <c r="E16" s="17">
+        <v>2.44</v>
+      </c>
+      <c r="F16" s="19">
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="14"/>
-      <c r="F17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
@@ -862,7 +909,8 @@
       <c r="D19" s="9">
         <v>2887</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -877,17 +925,20 @@
       <c r="D20" s="9">
         <v>120</v>
       </c>
-      <c r="F20" s="11">
-        <v>0.01</v>
+      <c r="E20" s="16">
+        <v>2.37</v>
+      </c>
+      <c r="F20" s="18">
+        <v>125.65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -896,8 +947,11 @@
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Effect size properly reversed, tables updated with values. Code may be ready.
</commit_message>
<xml_diff>
--- a/Table3_Adachi-and-others.xlsx
+++ b/Table3_Adachi-and-others.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Variable and study</t>
   </si>
@@ -43,21 +43,6 @@
   </si>
   <si>
     <t>[.02, .39]</t>
-  </si>
-  <si>
-    <r>
-      <t>Time (pre-, post-) X Game (Red Dead Redemption, FIFA)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> </t>
-    </r>
   </si>
   <si>
     <t>Przybylski et al., 2014, Study 1</t>
@@ -152,11 +137,77 @@
   <si>
     <t>BF02</t>
   </si>
+  <si>
+    <r>
+      <t>Time (pre-, post-) X Game (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Red Dead Redemption</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FIFA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Note: Might need to add mention of study designs, # groups, etc.</t>
+  </si>
+  <si>
+    <t>Figure out formatting for subscripts within column headings; alignment of column headings and values</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode=".00"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -269,28 +320,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,24 +681,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>0.28999999999999998</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -643,23 +707,23 @@
       <c r="D3" s="9">
         <v>2513</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="24">
         <v>0.22</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="17">
         <v>100</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="21">
         <v>0.44</v>
       </c>
       <c r="F4" s="19">
@@ -667,212 +731,213 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="17"/>
+      <c r="A5" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>11</v>
       </c>
       <c r="D6" s="9">
         <v>99</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="14">
         <v>2.97</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="15">
         <v>62.8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="23">
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="D7" s="9">
         <v>101</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="14">
         <v>2.34</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="15">
         <v>7.05</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.13</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0.13</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="D8" s="9">
         <v>120</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="14">
         <v>1.44</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="15">
         <v>1.82</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="23">
         <v>0.21</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="9">
         <v>1454</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="D11" s="9">
         <v>84</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="14">
         <v>0.79</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="15">
         <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="23">
+        <v>0.11</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="9">
-        <v>0.11</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="9">
         <v>84</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="14">
         <v>1.93</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="15">
         <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="D13" s="9">
         <v>50</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="14">
         <v>2.3199999999999998</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="15">
         <v>2.35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="9">
-        <v>0.01</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>25</v>
       </c>
       <c r="D14" s="9">
         <v>77</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="14">
         <v>2.7</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="15">
         <v>4.37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="23">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="D15" s="9">
         <v>42</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="14">
         <v>2.21</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="15">
         <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="24">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="13">
-        <v>0.03</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="D16" s="17">
         <v>60</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="20">
         <v>2.44</v>
       </c>
       <c r="F16" s="19">
@@ -881,60 +946,71 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="17"/>
+        <v>29</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="20"/>
+        <v>30</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="23">
         <v>0.22</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="9">
         <v>2887</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="20"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="9">
+        <v>13</v>
+      </c>
+      <c r="B20" s="23">
         <v>-0.08</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="9">
         <v>120</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="14">
         <v>2.37</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="15">
         <v>125.65</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top-to-bottom once-thru. Code updated to include aggressive behavior (tangram hurting) from Tear and Nielsen 2014.
</commit_message>
<xml_diff>
--- a/Table3_Adachi-and-others.xlsx
+++ b/Table3_Adachi-and-others.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Variable and study</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>Figure out formatting for subscripts within column headings; alignment of column headings and values</t>
+  </si>
+  <si>
+    <t>Przybylski et al., 2014, Study 5</t>
+  </si>
+  <si>
+    <t>[-.16, .22]</t>
+  </si>
+  <si>
+    <t>Tear &amp; Nielsen, 2014; Violent &amp; Ultraviolent conditions combined</t>
+  </si>
+  <si>
+    <t>Tear &amp; Nielsen, 2014, hurting behavior in Tangram task</t>
+  </si>
+  <si>
+    <t>[-.17, .19]</t>
   </si>
 </sst>
 </file>
@@ -282,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,19 +357,31 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,15 +683,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -698,7 +725,7 @@
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>0.28999999999999998</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -714,37 +741,37 @@
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="25">
         <v>0.22</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="27">
         <v>100</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="29">
         <v>0.44</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="28">
         <v>0.12</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="19"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="28"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>0</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -754,7 +781,7 @@
         <v>99</v>
       </c>
       <c r="E6" s="14">
-        <v>2.97</v>
+        <v>2.96</v>
       </c>
       <c r="F6" s="15">
         <v>62.8</v>
@@ -764,7 +791,7 @@
       <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>0.08</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -774,7 +801,7 @@
         <v>101</v>
       </c>
       <c r="E7" s="14">
-        <v>2.34</v>
+        <v>2.35</v>
       </c>
       <c r="F7" s="15">
         <v>7.05</v>
@@ -782,235 +809,280 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="17">
+        <v>109</v>
+      </c>
+      <c r="E8" s="20">
+        <v>2.96</v>
+      </c>
+      <c r="F8" s="19">
+        <v>38.119999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B9" s="22">
         <v>0.13</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D9" s="9">
         <v>120</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E9" s="14">
         <v>1.44</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F9" s="15">
         <v>1.82</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="23">
-        <v>0.21</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="9">
-        <v>1454</v>
-      </c>
+      <c r="B10" s="24"/>
       <c r="E10" s="14"/>
       <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="23">
-        <v>0.2</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="22">
+        <v>0.21</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="9">
-        <v>84</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0.79</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0.2</v>
-      </c>
+        <v>1454</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="23">
-        <v>0.11</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="22">
+        <v>0.2</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9">
         <v>84</v>
       </c>
       <c r="E12" s="14">
-        <v>1.93</v>
+        <v>0.79</v>
       </c>
       <c r="F12" s="15">
-        <v>0.94</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="23">
-        <v>0.02</v>
+        <v>19</v>
+      </c>
+      <c r="B13" s="22">
+        <v>0.11</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="9">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="E13" s="14">
-        <v>2.3199999999999998</v>
+        <v>1.93</v>
       </c>
       <c r="F13" s="15">
-        <v>2.35</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="23">
-        <v>0.01</v>
+        <v>21</v>
+      </c>
+      <c r="B14" s="22">
+        <v>0.02</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="9">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="E14" s="14">
-        <v>2.7</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="F14" s="15">
-        <v>4.37</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="23">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="22">
+        <v>0.01</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="9">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E15" s="14">
-        <v>2.21</v>
+        <v>2.7</v>
       </c>
       <c r="F15" s="15">
-        <v>2.4</v>
+        <v>4.37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="22">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="9">
+        <v>42</v>
+      </c>
+      <c r="E16" s="14">
+        <v>2.21</v>
+      </c>
+      <c r="F16" s="15">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B17" s="25">
         <v>0.03</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C17" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D17" s="27">
         <v>60</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E17" s="29">
         <v>2.44</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F17" s="28">
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="B18" s="25"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="16"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="17">
+        <v>120</v>
+      </c>
+      <c r="E19" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="F19" s="19">
+        <v>9.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B21" s="22">
         <v>0.22</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D21" s="9">
         <v>2887</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="16"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B22" s="22">
         <v>-0.08</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D22" s="9">
         <v>120</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E22" s="14">
         <v>2.37</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F22" s="15">
         <v>125.65</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1019,12 +1091,12 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="F4:F5"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F18"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>